<commit_message>
Resolved item in 3, 7 in issue #25
</commit_message>
<xml_diff>
--- a/tests/sample.xlsx
+++ b/tests/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amody/tetramer_validator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amody/tetramer-validator/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B959B7-6DC6-F24C-9A28-B74D7056BF1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058E4DD0-6CF6-174C-A29D-3E4D0C8B7DF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="2800" windowWidth="26840" windowHeight="15940" xr2:uid="{75EA4563-2D60-EC4A-8450-2866E5CE21DF}"/>
+    <workbookView xWindow="11780" yWindow="3320" windowWidth="26840" windowHeight="15940" xr2:uid="{75EA4563-2D60-EC4A-8450-2866E5CE21DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>PKYVKQNTLKLAT</t>
   </si>
   <si>
-    <t>OX</t>
-  </si>
-  <si>
     <t>M5</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>oxidation</t>
+  </si>
+  <si>
+    <t>oxidized residue</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70ED2FBD-23AD-F24A-9FED-5768149E1ABF}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -454,27 +456,27 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="F3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Rearranged order of columns in test files.
</commit_message>
<xml_diff>
--- a/tests/sample.xlsx
+++ b/tests/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amody/tetramer-validator/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058E4DD0-6CF6-174C-A29D-3E4D0C8B7DF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7962C9B7-679A-ED41-861F-531655D8245A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11780" yWindow="3320" windowWidth="26840" windowHeight="15940" xr2:uid="{75EA4563-2D60-EC4A-8450-2866E5CE21DF}"/>
+    <workbookView xWindow="9000" yWindow="3320" windowWidth="26840" windowHeight="15940" xr2:uid="{75EA4563-2D60-EC4A-8450-2866E5CE21DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Modification Position</t>
   </si>
   <si>
-    <t>MHC Name</t>
-  </si>
-  <si>
     <t>PKYVKQNTLKLAT</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>oxidized residue</t>
+  </si>
+  <si>
+    <t>MHC Molecule</t>
   </si>
 </sst>
 </file>
@@ -432,51 +432,51 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" s="2"/>
     </row>

</xml_diff>